<commit_message>
Actualización 5 dominios C
</commit_message>
<xml_diff>
--- a/PRODUCTOS/TAMANIO/Tam_Total.xlsx
+++ b/PRODUCTOS/TAMANIO/Tam_Total.xlsx
@@ -536,13 +536,13 @@
         <v>116</v>
       </c>
       <c r="C2" t="n">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="D2" t="n">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="E2" t="n">
-        <v>65</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3">
@@ -553,13 +553,13 @@
         <v>213</v>
       </c>
       <c r="C3" t="n">
-        <v>91</v>
+        <v>154</v>
       </c>
       <c r="D3" t="n">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="E3" t="n">
-        <v>91</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4">
@@ -570,13 +570,13 @@
         <v>2281</v>
       </c>
       <c r="C4" t="n">
-        <v>138</v>
+        <v>235</v>
       </c>
       <c r="D4" t="n">
-        <v>138</v>
+        <v>183</v>
       </c>
       <c r="E4" t="n">
-        <v>138</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5">
@@ -587,13 +587,13 @@
         <v>31</v>
       </c>
       <c r="C5" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D5" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E5" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
@@ -621,13 +621,13 @@
         <v>113</v>
       </c>
       <c r="C7" t="n">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="D7" t="n">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="E7" t="n">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8">
@@ -638,13 +638,13 @@
         <v>77</v>
       </c>
       <c r="C8" t="n">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="D8" t="n">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="E8" t="n">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9">
@@ -655,13 +655,13 @@
         <v>87</v>
       </c>
       <c r="C9" t="n">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="D9" t="n">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E9" t="n">
-        <v>57</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10">
@@ -672,13 +672,13 @@
         <v>21</v>
       </c>
       <c r="C10" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D10" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E10" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
@@ -689,13 +689,13 @@
         <v>225</v>
       </c>
       <c r="C11" t="n">
-        <v>85</v>
+        <v>138</v>
       </c>
       <c r="D11" t="n">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="E11" t="n">
-        <v>85</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12">
@@ -706,13 +706,13 @@
         <v>523</v>
       </c>
       <c r="C12" t="n">
-        <v>118</v>
+        <v>239</v>
       </c>
       <c r="D12" t="n">
-        <v>118</v>
+        <v>179</v>
       </c>
       <c r="E12" t="n">
-        <v>118</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13">
@@ -723,13 +723,13 @@
         <v>219</v>
       </c>
       <c r="C13" t="n">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="D13" t="n">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="E13" t="n">
-        <v>80</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14">
@@ -740,13 +740,13 @@
         <v>45</v>
       </c>
       <c r="C14" t="n">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D14" t="n">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E14" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15">
@@ -757,13 +757,13 @@
         <v>22</v>
       </c>
       <c r="C15" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D15" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E15" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16">
@@ -774,13 +774,13 @@
         <v>39</v>
       </c>
       <c r="C16" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D16" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E16" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17">
@@ -1000,13 +1000,13 @@
         <v>43</v>
       </c>
       <c r="C30" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D30" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E30" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31">

</xml_diff>